<commit_message>
fixed #33 TournRPG-33 アイテム一覧の表示
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -63,7 +63,7 @@
     <t>str</t>
   </si>
   <si>
-    <t>POTION1</t>
+    <t>POTION01</t>
   </si>
   <si>
     <t>Potion</t>
@@ -75,7 +75,7 @@
     <t>飲むとHPが10回復します</t>
   </si>
   <si>
-    <t>POTION2</t>
+    <t>POTION02</t>
   </si>
   <si>
     <t>回復薬20</t>
@@ -84,7 +84,7 @@
     <t>飲むとHPが20回復します</t>
   </si>
   <si>
-    <t>POTION3</t>
+    <t>POTION03</t>
   </si>
   <si>
     <t>回復薬30</t>
@@ -93,7 +93,7 @@
     <t>飲むとHPが30回復します</t>
   </si>
   <si>
-    <t>POTION4</t>
+    <t>POTION04</t>
   </si>
   <si>
     <t>回復薬40</t>
@@ -102,7 +102,7 @@
     <t>飲むとHPが40回復します</t>
   </si>
   <si>
-    <t>POTION5</t>
+    <t>POTION05</t>
   </si>
   <si>
     <t>回復薬50</t>
@@ -111,7 +111,7 @@
     <t>飲むとHPが50回復します</t>
   </si>
   <si>
-    <t>POTION6</t>
+    <t>POTION06</t>
   </si>
   <si>
     <t>回復薬60</t>
@@ -120,7 +120,7 @@
     <t>飲むとHPが60回復します</t>
   </si>
   <si>
-    <t>POTION7</t>
+    <t>POTION07</t>
   </si>
   <si>
     <t>回復薬70</t>
@@ -129,7 +129,7 @@
     <t>飲むとHPが70回復します</t>
   </si>
   <si>
-    <t>POTION8</t>
+    <t>POTION08</t>
   </si>
   <si>
     <t>回復薬80</t>
@@ -147,7 +147,7 @@
     <t>ext_val</t>
   </si>
   <si>
-    <t>WEAPON1</t>
+    <t>WEAPON01</t>
   </si>
   <si>
     <t>Weapon</t>
@@ -159,7 +159,7 @@
     <t>ただの木の棒。攻撃力2</t>
   </si>
   <si>
-    <t>WEAPON2</t>
+    <t>WEAPON02</t>
   </si>
   <si>
     <t>木刀</t>
@@ -168,7 +168,7 @@
     <t>木で作られた刀。攻撃力4</t>
   </si>
   <si>
-    <t>WEAPON3</t>
+    <t>WEAPON03</t>
   </si>
   <si>
     <t>ダガー</t>
@@ -177,7 +177,7 @@
     <t>小型の刃物。攻撃力6</t>
   </si>
   <si>
-    <t>WEAPON4</t>
+    <t>WEAPON04</t>
   </si>
   <si>
     <t>レイピア</t>
@@ -186,7 +186,7 @@
     <t>細身の剣。攻撃力10</t>
   </si>
   <si>
-    <t>WEAPON5</t>
+    <t>WEAPON05</t>
   </si>
   <si>
     <t>三日月刀</t>
@@ -195,7 +195,7 @@
     <t>よく切れる刀。攻撃力14</t>
   </si>
   <si>
-    <t>WEAPON6</t>
+    <t>WEAPON06</t>
   </si>
   <si>
     <t>妖刀ムラマサ</t>
@@ -204,7 +204,7 @@
     <t>妖気を帯びた刀。攻撃力16</t>
   </si>
   <si>
-    <t>WEAPON7</t>
+    <t>WEAPON07</t>
   </si>
   <si>
     <t>聖騎士の剣</t>
@@ -213,7 +213,7 @@
     <t>聖なる祝福を受けた剣。攻撃力20</t>
   </si>
   <si>
-    <t>WEAPON8</t>
+    <t>WEAPON08</t>
   </si>
   <si>
     <t>ドリル</t>
@@ -225,7 +225,7 @@
     <t>壁を壊せる武器。一定回数で壊れる。攻撃力5</t>
   </si>
   <si>
-    <t>ARMOR1</t>
+    <t>ARMOR01</t>
   </si>
   <si>
     <t>Armor</t>
@@ -237,7 +237,7 @@
     <t>敵の攻撃を少しだけ防ぐ衣服。防御力2</t>
   </si>
   <si>
-    <t>ARMOR2</t>
+    <t>ARMOR02</t>
   </si>
   <si>
     <t>毛皮の鎧</t>
@@ -246,7 +246,7 @@
     <t>丈夫な皮で作られた鎧。防御力4</t>
   </si>
   <si>
-    <t>ARMOR3</t>
+    <t>ARMOR03</t>
   </si>
   <si>
     <t>鎖かたびら</t>
@@ -255,7 +255,7 @@
     <t>鎖を編んで作られた鎧。防御力6</t>
   </si>
   <si>
-    <t>ARMOR4</t>
+    <t>ARMOR04</t>
   </si>
   <si>
     <t>エルフの鎧</t>
@@ -264,7 +264,7 @@
     <t>エルフが身につける鎧。防御力10</t>
   </si>
   <si>
-    <t>ARMOR5</t>
+    <t>ARMOR05</t>
   </si>
   <si>
     <t>メタルアーマー</t>
@@ -273,7 +273,7 @@
     <t>鋼で作られた丈夫な鎧。防御力14</t>
   </si>
   <si>
-    <t>ARMOR6</t>
+    <t>ARMOR06</t>
   </si>
   <si>
     <t>銀のジャケット</t>
@@ -282,7 +282,7 @@
     <t>魔法の銀で作られた防具。防御力16</t>
   </si>
   <si>
-    <t>ARMOR7</t>
+    <t>ARMOR07</t>
   </si>
   <si>
     <t>プラチナメイル</t>
@@ -291,7 +291,7 @@
     <t>プラチナ製の強力な鎧。防御力20</t>
   </si>
   <si>
-    <t>ARMOR8</t>
+    <t>ARMOR08</t>
   </si>
   <si>
     <t>反撃の鎧</t>
@@ -303,7 +303,7 @@
     <t>敵の攻撃で受けたダメージを相手に少し与える鎧。防御力10</t>
   </si>
   <si>
-    <t>RING1</t>
+    <t>RING01</t>
   </si>
   <si>
     <t>Ring</t>
@@ -315,7 +315,7 @@
     <t>力が1ポイント上昇します</t>
   </si>
   <si>
-    <t>RING2</t>
+    <t>RING02</t>
   </si>
   <si>
     <t>守りの指輪</t>
@@ -324,7 +324,7 @@
     <t>敵からのダメージを少し減らします</t>
   </si>
   <si>
-    <t>RING3</t>
+    <t>RING03</t>
   </si>
   <si>
     <t>HP増加の指輪</t>
@@ -336,7 +336,7 @@
     <t>最大HPが10上昇します</t>
   </si>
   <si>
-    <t>RING4</t>
+    <t>RING04</t>
   </si>
   <si>
     <t>眠りよけの指輪</t>
@@ -348,7 +348,7 @@
     <t>眠り状態を防ぎます</t>
   </si>
   <si>
-    <t>RING5</t>
+    <t>RING05</t>
   </si>
   <si>
     <t>混乱よけの指輪</t>
@@ -360,7 +360,7 @@
     <t>混乱状態を防ぎます</t>
   </si>
   <si>
-    <t>RING6</t>
+    <t>RING06</t>
   </si>
   <si>
     <t>通過の指輪</t>
@@ -372,7 +372,7 @@
     <t>水たまりを移動できるようになります</t>
   </si>
   <si>
-    <t>RING7</t>
+    <t>RING07</t>
   </si>
   <si>
     <t>力の指輪+1</t>
@@ -381,7 +381,7 @@
     <t>力が2ポイント上昇します</t>
   </si>
   <si>
-    <t>RING8</t>
+    <t>RING08</t>
   </si>
   <si>
     <t>力の指輪+2</t>
@@ -1769,7 +1769,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.9844" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
fixed #266 TournRPG-266 アイテムデータの作成
</commit_message>
<xml_diff>
--- a/docs/item.xlsx
+++ b/docs/item.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
   <si>
     <t>id</t>
   </si>
@@ -63,19 +63,148 @@
     <t>Potion</t>
   </si>
   <si>
+    <t>水</t>
+  </si>
+  <si>
+    <t>HPが5回復します</t>
+  </si>
+  <si>
+    <t>POTION02</t>
+  </si>
+  <si>
+    <t>おいしい水</t>
+  </si>
+  <si>
+    <t>HPが10回復します</t>
+  </si>
+  <si>
+    <t>POTION03</t>
+  </si>
+  <si>
+    <t>回復薬50</t>
+  </si>
+  <si>
+    <t>HPが50回復します</t>
+  </si>
+  <si>
+    <t>POTION04</t>
+  </si>
+  <si>
+    <t>命の水</t>
+  </si>
+  <si>
+    <t>hpmax</t>
+  </si>
+  <si>
+    <t>最大HPが上昇します</t>
+  </si>
+  <si>
+    <t>POTION05</t>
+  </si>
+  <si>
+    <t>力の薬</t>
+  </si>
+  <si>
+    <t>力が上昇します</t>
+  </si>
+  <si>
+    <t>POTION06</t>
+  </si>
+  <si>
+    <t>体力の薬</t>
+  </si>
+  <si>
+    <t>vit</t>
+  </si>
+  <si>
+    <t>体力が上昇します</t>
+  </si>
+  <si>
+    <t>POTION07</t>
+  </si>
+  <si>
+    <t>素早さの薬</t>
+  </si>
+  <si>
+    <t>agi</t>
+  </si>
+  <si>
+    <t>素早さが上昇します</t>
+  </si>
+  <si>
+    <t>POTION08</t>
+  </si>
+  <si>
+    <t>魔力の薬</t>
+  </si>
+  <si>
+    <t>mag</t>
+  </si>
+  <si>
+    <t>魔力が上昇します</t>
+  </si>
+  <si>
+    <t>POTION09</t>
+  </si>
+  <si>
+    <t>回復薬10</t>
+  </si>
+  <si>
+    <t>POTION10</t>
+  </si>
+  <si>
+    <t>回復薬20</t>
+  </si>
+  <si>
+    <t>HPが20回復します</t>
+  </si>
+  <si>
+    <t>POTION11</t>
+  </si>
+  <si>
     <t>回復薬30</t>
   </si>
   <si>
-    <t>飲むとHPが30回復します</t>
-  </si>
-  <si>
-    <t>POTION02</t>
-  </si>
-  <si>
-    <t>回復薬50</t>
-  </si>
-  <si>
-    <t>飲むとHPが50回復します</t>
+    <t>HPが30回復します</t>
+  </si>
+  <si>
+    <t>POTION12</t>
+  </si>
+  <si>
+    <t>回復薬40</t>
+  </si>
+  <si>
+    <t>HPが40回復します</t>
+  </si>
+  <si>
+    <t>POTION13</t>
+  </si>
+  <si>
+    <t>POTION14</t>
+  </si>
+  <si>
+    <t>回復薬60</t>
+  </si>
+  <si>
+    <t>HPが60回復します</t>
+  </si>
+  <si>
+    <t>POTION15</t>
+  </si>
+  <si>
+    <t>回復薬70</t>
+  </si>
+  <si>
+    <t>HPが70回復します</t>
+  </si>
+  <si>
+    <t>POTION16</t>
+  </si>
+  <si>
+    <t>回復薬80</t>
+  </si>
+  <si>
+    <t>HPが80回復します</t>
   </si>
   <si>
     <t>def</t>
@@ -274,9 +403,6 @@
   </si>
   <si>
     <t>HP増加の指輪</t>
-  </si>
-  <si>
-    <t>hpmax</t>
   </si>
   <si>
     <t>最大HPが10上昇します</t>
@@ -343,11 +469,11 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -374,11 +500,6 @@
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -400,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -423,59 +544,38 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -500,7 +600,6 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -559,53 +658,8 @@
         <a:cs typeface="ヒラギノ角ゴ ProN W3"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Blank">
       <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="129999"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -674,27 +728,6 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="104999"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
@@ -724,83 +757,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -871,12 +829,13 @@
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1165,6 +1124,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -1446,12 +1406,13 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1732,27 +1693,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
+      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.9844" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="4" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4" style="1" customWidth="1"/>
-    <col min="11" max="11" width="3.375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31.2812" style="1" customWidth="1"/>
-    <col min="13" max="256" width="9" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.17188" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.9688" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.35156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.35156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.35156" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.35156" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.35156" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="41.6875" style="1" customWidth="1"/>
+    <col min="13" max="256" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -1841,21 +1802,21 @@
       <c r="C3" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="D3" s="5">
-        <v>30</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6">
-        <v>20</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="D3" s="6">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7">
+        <v>10</v>
+      </c>
+      <c r="J3" s="7">
         <f>I3*0.35</f>
-        <v>7</v>
-      </c>
-      <c r="K3" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="K3" s="7">
         <v>200</v>
       </c>
       <c r="L3" t="s" s="5">
@@ -1872,29 +1833,473 @@
       <c r="C4" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7">
+        <f>I4*0.35</f>
+        <v>8.75</v>
+      </c>
+      <c r="K4" s="7">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6">
         <v>50</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7">
+        <v>150</v>
+      </c>
+      <c r="J5" s="7">
+        <f>I5*0.35</f>
+        <v>52.5</v>
+      </c>
+      <c r="K5" s="7">
+        <v>202</v>
+      </c>
+      <c r="L5" t="s" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3</v>
+      </c>
+      <c r="I6" s="7">
+        <v>500</v>
+      </c>
+      <c r="J6" s="7">
+        <f>I6*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K6" s="7">
+        <v>203</v>
+      </c>
+      <c r="L6" t="s" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="7">
+        <f>I7*0.35</f>
+        <v>350</v>
+      </c>
+      <c r="K7" s="7">
+        <v>204</v>
+      </c>
+      <c r="L7" t="s" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="7">
+        <f>I8*0.35</f>
+        <v>350</v>
+      </c>
+      <c r="K8" s="7">
+        <v>205</v>
+      </c>
+      <c r="L8" t="s" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1000</v>
+      </c>
+      <c r="J9" s="7">
+        <f>I9*0.35</f>
+        <v>350</v>
+      </c>
+      <c r="K9" s="7">
+        <v>206</v>
+      </c>
+      <c r="L9" t="s" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" t="s" s="5">
+        <v>41</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1000</v>
+      </c>
+      <c r="J10" s="7">
+        <f>I10*0.35</f>
+        <v>350</v>
+      </c>
+      <c r="K10" s="7">
+        <v>207</v>
+      </c>
+      <c r="L10" t="s" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="D11" s="6">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7">
+        <v>500</v>
+      </c>
+      <c r="J11" s="7">
+        <f>I11*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K11" s="7">
+        <v>208</v>
+      </c>
+      <c r="L11" t="s" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="A12" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>46</v>
+      </c>
+      <c r="D12" s="6">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7">
+        <v>500</v>
+      </c>
+      <c r="J12" s="7">
+        <f>I12*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K12" s="7">
+        <v>209</v>
+      </c>
+      <c r="L12" t="s" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="D13" s="6">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="7">
+        <v>500</v>
+      </c>
+      <c r="J13" s="7">
+        <f>I13*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K13" s="7">
+        <v>210</v>
+      </c>
+      <c r="L13" t="s" s="5">
         <v>50</v>
       </c>
-      <c r="J4" s="9">
-        <f>I4*0.35</f>
-        <v>17.5</v>
-      </c>
-      <c r="K4" s="9">
-        <v>201</v>
-      </c>
-      <c r="L4" t="s" s="10">
-        <v>20</v>
+    </row>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>52</v>
+      </c>
+      <c r="D14" s="6">
+        <v>40</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="7">
+        <v>500</v>
+      </c>
+      <c r="J14" s="7">
+        <f>I14*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K14" s="7">
+        <v>211</v>
+      </c>
+      <c r="L14" t="s" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1">
+      <c r="A15" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D15" s="6">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7">
+        <v>500</v>
+      </c>
+      <c r="J15" s="7">
+        <f>I15*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K15" s="7">
+        <v>212</v>
+      </c>
+      <c r="L15" t="s" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>56</v>
+      </c>
+      <c r="D16" s="6">
+        <v>60</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7">
+        <v>500</v>
+      </c>
+      <c r="J16" s="7">
+        <f>I16*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K16" s="7">
+        <v>213</v>
+      </c>
+      <c r="L16" t="s" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>59</v>
+      </c>
+      <c r="D17" s="6">
+        <v>70</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="7">
+        <v>500</v>
+      </c>
+      <c r="J17" s="7">
+        <f>I17*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K17" s="7">
+        <v>214</v>
+      </c>
+      <c r="L17" t="s" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1">
+      <c r="A18" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s" s="5">
+        <v>62</v>
+      </c>
+      <c r="D18" s="6">
+        <v>80</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="7">
+        <v>500</v>
+      </c>
+      <c r="J18" s="7">
+        <f>I18*0.35</f>
+        <v>175</v>
+      </c>
+      <c r="K18" s="7">
+        <v>215</v>
+      </c>
+      <c r="L18" t="s" s="5">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
@@ -1911,23 +2316,23 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.1172" style="11" customWidth="1"/>
-    <col min="2" max="2" width="7.10938" style="11" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="11" customWidth="1"/>
-    <col min="4" max="4" width="3.125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="3.125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="3.125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="11" customWidth="1"/>
-    <col min="8" max="8" width="6" style="11" customWidth="1"/>
-    <col min="9" max="9" width="3.875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="4" style="11" customWidth="1"/>
-    <col min="11" max="11" width="4" style="11" customWidth="1"/>
-    <col min="12" max="12" width="3.375" style="11" customWidth="1"/>
-    <col min="13" max="13" width="34.75" style="11" customWidth="1"/>
-    <col min="14" max="14" width="2.75" style="11" customWidth="1"/>
-    <col min="15" max="256" width="12.25" style="11" customWidth="1"/>
+    <col min="1" max="1" width="13.4688" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.46875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="9" customWidth="1"/>
+    <col min="4" max="4" width="4.17188" style="9" customWidth="1"/>
+    <col min="5" max="5" width="4.17188" style="9" customWidth="1"/>
+    <col min="6" max="6" width="4.17188" style="9" customWidth="1"/>
+    <col min="7" max="7" width="9" style="9" customWidth="1"/>
+    <col min="8" max="8" width="8" style="9" customWidth="1"/>
+    <col min="9" max="9" width="5.17188" style="9" customWidth="1"/>
+    <col min="10" max="10" width="5.35156" style="9" customWidth="1"/>
+    <col min="11" max="11" width="5.35156" style="9" customWidth="1"/>
+    <col min="12" max="12" width="4.5" style="9" customWidth="1"/>
+    <col min="13" max="13" width="46.3516" style="9" customWidth="1"/>
+    <col min="14" max="14" width="3.67188" style="9" customWidth="1"/>
+    <col min="15" max="256" width="16.3516" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -1944,19 +2349,19 @@
         <v>4</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s" s="2">
         <v>8</v>
@@ -1971,7 +2376,7 @@
         <v>11</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -2020,870 +2425,870 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5">
+        <v>71</v>
+      </c>
+      <c r="D3" s="6">
         <v>2</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7">
         <v>50</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="7">
         <f>J3*0.35</f>
         <v>17.5</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="7">
         <v>100</v>
       </c>
       <c r="M3" t="s" s="5">
-        <v>29</v>
-      </c>
-      <c r="N3" s="6">
+        <v>72</v>
+      </c>
+      <c r="N3" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="D4" s="5">
+        <v>74</v>
+      </c>
+      <c r="D4" s="6">
         <v>5</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7">
         <v>100</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="7">
         <f>J4*0.35</f>
         <v>35</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="7">
         <v>101</v>
       </c>
       <c r="M4" t="s" s="5">
-        <v>32</v>
-      </c>
-      <c r="N4" s="6">
+        <v>75</v>
+      </c>
+      <c r="N4" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>34</v>
-      </c>
-      <c r="D5" s="5">
+        <v>77</v>
+      </c>
+      <c r="D5" s="6">
         <v>10</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7">
         <v>250</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="7">
         <f>J5*0.35</f>
         <v>87.5</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="7">
         <v>102</v>
       </c>
       <c r="M5" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="N5" s="6">
+        <v>78</v>
+      </c>
+      <c r="N5" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>37</v>
-      </c>
-      <c r="D6" s="5">
+        <v>80</v>
+      </c>
+      <c r="D6" s="6">
         <v>10</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
         <v>700</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="7">
         <f>J6*0.35</f>
         <v>245</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="7">
         <v>103</v>
       </c>
       <c r="M6" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="N6" s="6">
+        <v>81</v>
+      </c>
+      <c r="N6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s" s="5">
-        <v>40</v>
-      </c>
-      <c r="D7" s="5">
+        <v>83</v>
+      </c>
+      <c r="D7" s="6">
         <v>14</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7">
         <v>1000</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="7">
         <f>J7*0.35</f>
         <v>350</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="7">
         <v>104</v>
       </c>
       <c r="M7" t="s" s="5">
-        <v>41</v>
-      </c>
-      <c r="N7" s="6">
+        <v>84</v>
+      </c>
+      <c r="N7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="D8" s="5">
+        <v>86</v>
+      </c>
+      <c r="D8" s="6">
         <v>16</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7">
         <v>1500</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="7">
         <f>J8*0.35</f>
         <v>525</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="7">
         <v>105</v>
       </c>
       <c r="M8" t="s" s="5">
-        <v>44</v>
-      </c>
-      <c r="N8" s="6">
+        <v>87</v>
+      </c>
+      <c r="N8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>46</v>
-      </c>
-      <c r="D9" s="5">
+        <v>89</v>
+      </c>
+      <c r="D9" s="6">
         <v>20</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7">
         <v>3000</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="7">
         <f>J9*0.35</f>
         <v>1050</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="7">
         <v>106</v>
       </c>
       <c r="M9" t="s" s="5">
-        <v>47</v>
-      </c>
-      <c r="N9" s="6">
+        <v>90</v>
+      </c>
+      <c r="N9" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s" s="5">
-        <v>49</v>
-      </c>
-      <c r="D10" s="5">
+        <v>92</v>
+      </c>
+      <c r="D10" s="6">
         <v>5</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" t="s" s="5">
-        <v>50</v>
-      </c>
-      <c r="H10" s="6">
+        <v>93</v>
+      </c>
+      <c r="H10" s="7">
         <v>100</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6">
+      <c r="I10" s="7"/>
+      <c r="J10" s="7">
         <v>500</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="7">
         <f>J10*0.35</f>
         <v>175</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="7">
         <v>107</v>
       </c>
       <c r="M10" t="s" s="5">
-        <v>51</v>
-      </c>
-      <c r="N10" s="6">
+        <v>94</v>
+      </c>
+      <c r="N10" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s" s="5">
-        <v>54</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5">
+        <v>97</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6">
         <v>2</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
         <v>50</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="7">
         <f>J11*0.35</f>
         <v>17.5</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="7">
         <v>120</v>
       </c>
       <c r="M11" t="s" s="5">
-        <v>55</v>
-      </c>
-      <c r="N11" s="5">
+        <v>98</v>
+      </c>
+      <c r="N11" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s" s="5">
-        <v>57</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5">
+        <v>100</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6">
         <v>5</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
         <v>100</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="7">
         <f>J12*0.35</f>
         <v>35</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="7">
         <v>121</v>
       </c>
       <c r="M12" t="s" s="5">
-        <v>58</v>
-      </c>
-      <c r="N12" s="5">
+        <v>101</v>
+      </c>
+      <c r="N12" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s" s="5">
-        <v>60</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5">
+        <v>103</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6">
         <v>10</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5">
-        <v>1</v>
-      </c>
-      <c r="J13" s="6">
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
         <v>250</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="7">
         <f>J13*0.35</f>
         <v>87.5</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="7">
         <v>122</v>
       </c>
       <c r="M13" t="s" s="5">
-        <v>61</v>
-      </c>
-      <c r="N13" s="5">
+        <v>104</v>
+      </c>
+      <c r="N13" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s" s="5">
-        <v>63</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5">
+        <v>106</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6">
         <v>10</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5">
-        <v>1</v>
-      </c>
-      <c r="J14" s="6">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
         <v>700</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="7">
         <f>J14*0.35</f>
         <v>245</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="7">
         <v>123</v>
       </c>
       <c r="M14" t="s" s="5">
-        <v>64</v>
-      </c>
-      <c r="N14" s="5">
+        <v>107</v>
+      </c>
+      <c r="N14" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>66</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5">
+        <v>109</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="6">
         <v>14</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="5">
-        <v>1</v>
-      </c>
-      <c r="J15" s="6">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7">
         <v>1000</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="7">
         <f>J15*0.35</f>
         <v>350</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="7">
         <v>124</v>
       </c>
       <c r="M15" t="s" s="5">
-        <v>67</v>
-      </c>
-      <c r="N15" s="5">
+        <v>110</v>
+      </c>
+      <c r="N15" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s" s="5">
-        <v>69</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5">
+        <v>112</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="6">
         <v>16</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5">
-        <v>1</v>
-      </c>
-      <c r="J16" s="6">
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
         <v>1500</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="7">
         <f>J16*0.35</f>
         <v>525</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="7">
         <v>125</v>
       </c>
       <c r="M16" t="s" s="5">
-        <v>70</v>
-      </c>
-      <c r="N16" s="5">
+        <v>113</v>
+      </c>
+      <c r="N16" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s" s="5">
-        <v>72</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5">
+        <v>115</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6">
         <v>20</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5">
-        <v>1</v>
-      </c>
-      <c r="J17" s="6">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7">
         <v>3000</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="7">
         <f>J17*0.35</f>
         <v>1050</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="7">
         <v>126</v>
       </c>
       <c r="M17" t="s" s="5">
-        <v>73</v>
-      </c>
-      <c r="N17" s="5">
+        <v>116</v>
+      </c>
+      <c r="N17" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s" s="5">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s" s="5">
-        <v>75</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5">
+        <v>118</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="6">
         <v>10</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="7"/>
       <c r="G18" t="s" s="5">
-        <v>76</v>
-      </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="5">
-        <v>1</v>
-      </c>
-      <c r="J18" s="6">
+        <v>119</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="6">
+        <v>1</v>
+      </c>
+      <c r="J18" s="7">
         <v>2000</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="7">
         <f>J18*0.35</f>
         <v>700</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="7">
         <v>127</v>
       </c>
       <c r="M18" t="s" s="5">
-        <v>77</v>
-      </c>
-      <c r="N18" s="5">
+        <v>120</v>
+      </c>
+      <c r="N18" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s" s="5">
-        <v>80</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="6">
+        <v>123</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="7">
         <v>300</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="7">
         <f>J19*0.35</f>
         <v>105</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="7">
         <v>140</v>
       </c>
       <c r="M19" t="s" s="5">
-        <v>81</v>
-      </c>
-      <c r="N19" s="5">
+        <v>124</v>
+      </c>
+      <c r="N19" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C20" t="s" s="5">
-        <v>83</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="6">
+        <v>126</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="7">
         <v>300</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="7">
         <f>J20*0.35</f>
         <v>105</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="7">
         <v>141</v>
       </c>
       <c r="M20" t="s" s="5">
-        <v>84</v>
-      </c>
-      <c r="N20" s="5">
+        <v>127</v>
+      </c>
+      <c r="N20" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s" s="5">
-        <v>86</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="6"/>
+        <v>129</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
       <c r="G21" t="s" s="5">
-        <v>87</v>
-      </c>
-      <c r="H21" s="6">
+        <v>26</v>
+      </c>
+      <c r="H21" s="7">
         <v>10</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="6">
+      <c r="I21" s="8"/>
+      <c r="J21" s="7">
         <v>300</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="7">
         <f>J21*0.35</f>
         <v>105</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="7">
         <v>142</v>
       </c>
       <c r="M21" t="s" s="5">
-        <v>88</v>
-      </c>
-      <c r="N21" s="5">
+        <v>130</v>
+      </c>
+      <c r="N21" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s" s="5">
-        <v>90</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6"/>
+        <v>132</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
       <c r="G22" t="s" s="5">
-        <v>91</v>
-      </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="6">
+        <v>133</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="7">
         <v>2000</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="7">
         <f>J22*0.35</f>
         <v>700</v>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="7">
         <v>143</v>
       </c>
       <c r="M22" t="s" s="5">
-        <v>92</v>
-      </c>
-      <c r="N22" s="5">
+        <v>134</v>
+      </c>
+      <c r="N22" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="B23" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s" s="5">
-        <v>94</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="6"/>
+        <v>136</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7"/>
       <c r="G23" t="s" s="5">
-        <v>95</v>
-      </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="6">
+        <v>137</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="7">
         <v>2000</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="7">
         <f>J23*0.35</f>
         <v>700</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="7">
         <v>144</v>
       </c>
       <c r="M23" t="s" s="5">
-        <v>96</v>
-      </c>
-      <c r="N23" s="5">
+        <v>138</v>
+      </c>
+      <c r="N23" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s" s="5">
-        <v>98</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="6"/>
+        <v>140</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
       <c r="G24" t="s" s="5">
-        <v>99</v>
-      </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="6">
+        <v>141</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="7">
         <v>2500</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="7">
         <f>J24*0.35</f>
         <v>875</v>
       </c>
-      <c r="L24" s="6">
+      <c r="L24" s="7">
         <v>145</v>
       </c>
       <c r="M24" t="s" s="5">
-        <v>100</v>
-      </c>
-      <c r="N24" s="5">
+        <v>142</v>
+      </c>
+      <c r="N24" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s" s="5">
-        <v>102</v>
-      </c>
-      <c r="D25" s="6">
+        <v>144</v>
+      </c>
+      <c r="D25" s="7">
         <v>2</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="6">
+      <c r="E25" s="8"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="7">
         <v>500</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="7">
         <f>J25*0.35</f>
         <v>175</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="7">
         <v>146</v>
       </c>
       <c r="M25" t="s" s="5">
-        <v>103</v>
-      </c>
-      <c r="N25" s="5">
+        <v>145</v>
+      </c>
+      <c r="N25" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s" s="5">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C26" t="s" s="5">
-        <v>105</v>
-      </c>
-      <c r="D26" s="6">
+        <v>147</v>
+      </c>
+      <c r="D26" s="7">
         <v>3</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="6">
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="7">
         <v>1000</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26" s="7">
         <f>J26*0.35</f>
         <v>350</v>
       </c>
-      <c r="L26" s="6">
+      <c r="L26" s="7">
         <v>147</v>
       </c>
       <c r="M26" t="s" s="5">
-        <v>106</v>
-      </c>
-      <c r="N26" s="5">
+        <v>148</v>
+      </c>
+      <c r="N26" s="6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>

</xml_diff>